<commit_message>
Anforderungsliste ergänzt, T-Tabelle mit Funktionen befüllt
</commit_message>
<xml_diff>
--- a/RB-Blessing/Anforderungsliste.xlsx
+++ b/RB-Blessing/Anforderungsliste.xlsx
@@ -1,25 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20340"/>
-  <workbookPr showInkAnnotation="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr showInkAnnotation="0" codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hopfm.tmb18\Documents\GitHub\KE3\RB-Blessing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anika\Documents\GitHub\KE3\RB-Blessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897EB3AA-4572-4EB6-955E-092CA1E41DB0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -28,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="129">
   <si>
     <t>Hauptmerkmal</t>
   </si>
@@ -234,9 +230,6 @@
     <t>Vorstellung der vollständigen Berechnungen und CAD-Zeichnungen</t>
   </si>
   <si>
-    <t>Abgabe der vollständigen Dokumentation</t>
-  </si>
-  <si>
     <t>Drehstrom</t>
   </si>
   <si>
@@ -246,9 +239,6 @@
     <t>keine Lebenszeitschmierung, aber Abdichtung der Lagergehäuse</t>
   </si>
   <si>
-    <t>Wälzlager, sollen Fluchtungs- und Montagefehler ausgleichen; keine überdimesionierte Lebensdauer (nicht &gt; 60000h)</t>
-  </si>
-  <si>
     <t>Kettentrieb</t>
   </si>
   <si>
@@ -322,9 +312,6 @@
   </si>
   <si>
     <t>8.2</t>
-  </si>
-  <si>
-    <t>8.3</t>
   </si>
   <si>
     <t>keine extreme Überschreitung der Lebensdauer</t>
@@ -381,11 +368,185 @@
   <si>
     <t>maximal 800€</t>
   </si>
+  <si>
+    <t>5.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aufstellen ohne Wartezeit </t>
+  </si>
+  <si>
+    <t>kein Einbetonieren der Stützen</t>
+  </si>
+  <si>
+    <t>Flexibilität</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anlage soll räumlich umbaubar sein, falls nötig </t>
+  </si>
+  <si>
+    <t>Sicherheit</t>
+  </si>
+  <si>
+    <t>9.1</t>
+  </si>
+  <si>
+    <t>9.2</t>
+  </si>
+  <si>
+    <t>9.3</t>
+  </si>
+  <si>
+    <t>Sicherung gegen herunterfallende Teile</t>
+  </si>
+  <si>
+    <t>Selbstzentrierendes Band</t>
+  </si>
+  <si>
+    <t>Sicherung gegen Hineinziehen von Gliedmaßen oder Gegenständen</t>
+  </si>
+  <si>
+    <t>Bedienung</t>
+  </si>
+  <si>
+    <t>Einschalten mit Einhandschalter</t>
+  </si>
+  <si>
+    <t>Nothalt mit Fußpedal</t>
+  </si>
+  <si>
+    <t>Abgabe der vollständigen Dokumentation in Papierform und auf CD</t>
+  </si>
+  <si>
+    <t>Staubige Umgebung</t>
+  </si>
+  <si>
+    <t>Keine Behinderung der Ketten oder sonstiger Teile durch Staub in der Umgebungsluft</t>
+  </si>
+  <si>
+    <t>Betriebsmittel</t>
+  </si>
+  <si>
+    <t>Fett</t>
+  </si>
+  <si>
+    <t>gleicher Typ wie in allen Anlagen von diesem Hersteller, die bisher ausgeliefert wurden</t>
+  </si>
+  <si>
+    <t>Kompletter Fettwechsel möglich</t>
+  </si>
+  <si>
+    <t>kein Fettsammelraum auf Lebenszeit</t>
+  </si>
+  <si>
+    <t>Keine Tropfenbildung durch Schmierfett</t>
+  </si>
+  <si>
+    <t>7.3</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>10.1</t>
+  </si>
+  <si>
+    <t>10.2</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>11.1</t>
+  </si>
+  <si>
+    <t>11.2</t>
+  </si>
+  <si>
+    <t>11.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forderung </t>
+  </si>
+  <si>
+    <t>6.3</t>
+  </si>
+  <si>
+    <t>Geräuscharm</t>
+  </si>
+  <si>
+    <t>&lt;70dB</t>
+  </si>
+  <si>
+    <t>7.4</t>
+  </si>
+  <si>
+    <t>Transportmaße</t>
+  </si>
+  <si>
+    <t>max. 800mmx800mmx800mm ohne Motor</t>
+  </si>
+  <si>
+    <t>ideal: Magnetlager; sonst Wälzlager, sollen Fluchtungs- und Montagefehler ausgleichen; keine überdimesionierte Lebensdauer (nicht &gt; 60000h)</t>
+  </si>
+  <si>
+    <t>6.4</t>
+  </si>
+  <si>
+    <t>Rostfrei</t>
+  </si>
+  <si>
+    <t>durch entsprechenden Werkstoff oder Beschichtung</t>
+  </si>
+  <si>
+    <t>6.5</t>
+  </si>
+  <si>
+    <t>Außenbetrieb möglich</t>
+  </si>
+  <si>
+    <t>5.3</t>
+  </si>
+  <si>
+    <t>Geringer Stromverbrauch</t>
+  </si>
+  <si>
+    <t>&lt;4kWh</t>
+  </si>
+  <si>
+    <t>6.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Netzbetrieb des Motors </t>
+  </si>
+  <si>
+    <t>ohne Trafo</t>
+  </si>
+  <si>
+    <t>6.7</t>
+  </si>
+  <si>
+    <t>Temperaturbereich</t>
+  </si>
+  <si>
+    <t>-10°C bis +40°C</t>
+  </si>
+  <si>
+    <t>1.6</t>
+  </si>
+  <si>
+    <t>Kompaktheit</t>
+  </si>
+  <si>
+    <t>Kettenlänge &lt;1000mm</t>
+  </si>
+  <si>
+    <t>Umgebung und Betriebsbedingungen</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -630,7 +791,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -682,38 +843,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -994,16 +1161,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Tabelle1"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.625" style="29" customWidth="1"/>
+    <col min="1" max="1" width="6.625" style="38" customWidth="1"/>
     <col min="2" max="2" width="25.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46.875" customWidth="1"/>
     <col min="4" max="4" width="13.125" customWidth="1"/>
@@ -1012,7 +1180,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="30" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="9" t="s">
@@ -1032,7 +1200,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24"/>
+      <c r="A2" s="31"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -1040,7 +1208,7 @@
       <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="30">
+      <c r="A3" s="32">
         <v>1</v>
       </c>
       <c r="B3" s="13" t="s">
@@ -1052,7 +1220,7 @@
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="33" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="15" t="s">
@@ -1064,11 +1232,11 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="33" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="15" t="s">
@@ -1080,11 +1248,11 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="33" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="15" t="s">
@@ -1096,469 +1264,807 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
-        <v>45</v>
+      <c r="A7" s="33" t="s">
+        <v>43</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="33" t="s">
-        <v>66</v>
+        <v>42</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>63</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
-        <v>46</v>
+      <c r="A8" s="33" t="s">
+        <v>44</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="31">
-        <v>2</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="15"/>
+      <c r="A9" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>127</v>
+      </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>33</v>
-      </c>
+      <c r="A10" s="34">
+        <v>2</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="15"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="2" t="s">
-        <v>71</v>
-      </c>
+      <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
-        <v>24</v>
+      <c r="A11" s="33" t="s">
+        <v>23</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
-        <v>39</v>
+      <c r="A12" s="33" t="s">
+        <v>24</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="31">
-        <v>3</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="15"/>
+      <c r="A13" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>36</v>
+      </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>36</v>
-      </c>
+      <c r="F13" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="34">
+        <v>3</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="15"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
-        <v>47</v>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="33" t="s">
+        <v>27</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>29</v>
+        <v>110</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>34</v>
+      <c r="A16" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>28</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="31">
-        <v>4</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="15"/>
+      <c r="A17" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>34</v>
+      </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="2"/>
+      <c r="F17" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="18" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>50</v>
-      </c>
+      <c r="A18" s="34">
+        <v>4</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="15"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="2" t="s">
-        <v>72</v>
-      </c>
+      <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="s">
-        <v>51</v>
+      <c r="A19" s="33" t="s">
+        <v>47</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="32">
-        <v>5</v>
-      </c>
-      <c r="B20" s="17" t="s">
+      <c r="A20" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="15"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="32">
+      <c r="F20" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="29" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="35">
+        <v>5</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="17"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="28"/>
+    </row>
+    <row r="22" spans="1:6" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="29" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="35">
         <v>6</v>
       </c>
-      <c r="B22" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="15"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="25" t="s">
+      <c r="B25" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="C25" s="17"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="28"/>
+    </row>
+    <row r="26" spans="1:6" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" s="18"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="B24" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="32">
+    </row>
+    <row r="29" spans="1:6" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="C30" s="18"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="C32" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="35">
         <v>7</v>
       </c>
-      <c r="B25" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="15"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="32">
-        <v>8</v>
-      </c>
-      <c r="B28" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" s="15"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="2"/>
-    </row>
-    <row r="29" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" s="19">
-        <v>43760</v>
-      </c>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A30" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C30" s="19">
-        <v>43781</v>
-      </c>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" s="19">
-        <v>43797</v>
-      </c>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="27"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="2"/>
-    </row>
-    <row r="33" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="27"/>
-      <c r="B33" s="15"/>
+      <c r="B33" s="17" t="s">
+        <v>51</v>
+      </c>
       <c r="C33" s="15"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="2"/>
     </row>
     <row r="34" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="27"/>
-      <c r="B34" s="15"/>
+      <c r="A34" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>55</v>
+      </c>
       <c r="C34" s="15"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
-      <c r="F34" s="2"/>
+      <c r="F34" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="35" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="27"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
+      <c r="A35" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>73</v>
+      </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
-      <c r="F35" s="2"/>
+      <c r="F35" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="36" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="27"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
+      <c r="A36" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="B36" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>75</v>
+      </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
-      <c r="F36" s="2"/>
+      <c r="F36" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="37" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="27"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
+      <c r="A37" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="B37" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>109</v>
+      </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
-      <c r="F37" s="2"/>
+      <c r="F37" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="38" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="27"/>
-      <c r="B38" s="15"/>
+      <c r="A38" s="35">
+        <v>6</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>52</v>
+      </c>
       <c r="C38" s="15"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="2"/>
     </row>
     <row r="39" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="27"/>
-      <c r="B39" s="15"/>
-      <c r="C39" s="15"/>
+      <c r="A39" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="B39" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>65</v>
+      </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
-      <c r="F39" s="2"/>
+      <c r="F39" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="40" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="27"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
+      <c r="A40" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>70</v>
+      </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
-      <c r="F40" s="2"/>
+      <c r="F40" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="41" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="27"/>
-      <c r="B41" s="20"/>
+      <c r="A41" s="35">
+        <v>8</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>15</v>
+      </c>
       <c r="C41" s="15"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="2"/>
     </row>
-    <row r="42" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="28"/>
-      <c r="B42" s="21"/>
-      <c r="C42" s="22"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="4"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C43" s="12"/>
+    <row r="42" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="29" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="35">
+        <v>9</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C44" s="17"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="28"/>
+    </row>
+    <row r="45" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C45" s="15"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C46" s="15"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A47" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C47" s="15"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="B48" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C48" s="17"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="27"/>
+      <c r="F48" s="28"/>
+    </row>
+    <row r="49" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A49" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C49" s="15"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="B50" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C50" s="15"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="29" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="B51" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C51" s="17"/>
+      <c r="D51" s="27"/>
+      <c r="E51" s="27"/>
+      <c r="F51" s="28"/>
+    </row>
+    <row r="52" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A52" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="B52" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C52" s="19">
+        <v>43760</v>
+      </c>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A53" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="B53" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C53" s="19">
+        <v>43781</v>
+      </c>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A54" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="B54" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C54" s="19">
+        <v>43797</v>
+      </c>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="36"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="2"/>
+    </row>
+    <row r="56" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="36"/>
+      <c r="B56" s="15"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="2"/>
+    </row>
+    <row r="57" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="36"/>
+      <c r="B57" s="15"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="2"/>
+    </row>
+    <row r="58" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="36"/>
+      <c r="B58" s="15"/>
+      <c r="C58" s="15"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="2"/>
+    </row>
+    <row r="59" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="36"/>
+      <c r="B59" s="15"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="2"/>
+    </row>
+    <row r="60" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="36"/>
+      <c r="B60" s="15"/>
+      <c r="C60" s="15"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="2"/>
+    </row>
+    <row r="61" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="36"/>
+      <c r="B61" s="15"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="2"/>
+    </row>
+    <row r="62" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="36"/>
+      <c r="B62" s="15"/>
+      <c r="C62" s="15"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="2"/>
+    </row>
+    <row r="63" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="36"/>
+      <c r="B63" s="15"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="2"/>
+    </row>
+    <row r="64" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="36"/>
+      <c r="B64" s="20"/>
+      <c r="C64" s="15"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="2"/>
+    </row>
+    <row r="65" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="37"/>
+      <c r="B65" s="21"/>
+      <c r="C65" s="22"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+      <c r="F65" s="4"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C66" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Formatierung Anforderungsliste und Paarweiser Vergleich
</commit_message>
<xml_diff>
--- a/RB-Blessing/Anforderungsliste.xlsx
+++ b/RB-Blessing/Anforderungsliste.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20340"/>
   <workbookPr showInkAnnotation="0" codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anika\Documents\GitHub\KE3\RB-Blessing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\langohra.tmb18\Documents\GitHub\KE3\RB-Blessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13A6FA1-9522-4ADF-84B0-8FFD32E211B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="130">
   <si>
     <t>Hauptmerkmal</t>
   </si>
@@ -542,11 +543,14 @@
   <si>
     <t>Umgebung und Betriebsbedingungen</t>
   </si>
+  <si>
+    <t>Wunsch/Forderung</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1161,22 +1165,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.625" style="38" customWidth="1"/>
     <col min="2" max="2" width="25.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.875" customWidth="1"/>
-    <col min="4" max="4" width="13.125" customWidth="1"/>
-    <col min="5" max="5" width="15.375" customWidth="1"/>
-    <col min="6" max="6" width="17.375" customWidth="1"/>
+    <col min="3" max="3" width="44.875" customWidth="1"/>
+    <col min="4" max="4" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.25" customWidth="1"/>
+    <col min="6" max="6" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1400,7 +1404,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="2" t="s">
-        <v>68</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -2068,8 +2072,8 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="69" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="10" r:id="rId1"/>
+  <pageMargins left="1.0236220472440944" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="69" orientation="portrait" copies="10" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"Calibri (Textkörper),Standard"&amp;14&amp;K00-034Produktspezifikation / Lastenheft&amp;C&amp;"Calibri (Textkörper),Fett"&amp;14&amp;K00-034Anforderungen&amp;R&amp;"Calibri (Textkörper),Standard"&amp;K00-034Version Nr. ____</oddHeader>
     <oddFooter>&amp;L&amp;"Calibri (Textkörper),Standard"&amp;K00-034Seite ____/_____&amp;C&amp;"Calibri (Textkörper),Standard"&amp;K00-034Heidenheim, den _________&amp;R&amp;"Calibri (Textkörper),Standard"&amp;K00-034erstellt von: ______________</oddFooter>

</xml_diff>

<commit_message>
Finale-Ordner erstellt, kleinere Änderungen
</commit_message>
<xml_diff>
--- a/RB-Blessing/Anforderungsliste.xlsx
+++ b/RB-Blessing/Anforderungsliste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\langohra.tmb18\Documents\GitHub\KE3\RB-Blessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13A6FA1-9522-4ADF-84B0-8FFD32E211B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094EE418-EAEF-4AE7-9CA8-DE12D5464970}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="134">
   <si>
     <t>Hauptmerkmal</t>
   </si>
   <si>
     <t>von wem</t>
-  </si>
-  <si>
-    <t>wann</t>
   </si>
   <si>
     <t>Klassifizierung</t>
@@ -545,6 +542,21 @@
   </si>
   <si>
     <t>Wunsch/Forderung</t>
+  </si>
+  <si>
+    <t>Frau Hopf</t>
+  </si>
+  <si>
+    <t>alle</t>
+  </si>
+  <si>
+    <t>Frau Langohr</t>
+  </si>
+  <si>
+    <t>Frau Hofmann</t>
+  </si>
+  <si>
+    <t>Herr Tiroch</t>
   </si>
 </sst>
 </file>
@@ -1167,10 +1179,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:F66"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1178,896 +1190,906 @@
     <col min="1" max="1" width="6.625" style="38" customWidth="1"/>
     <col min="2" max="2" width="25.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44.875" customWidth="1"/>
-    <col min="4" max="4" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.25" customWidth="1"/>
-    <col min="6" max="6" width="17.5" customWidth="1"/>
+    <col min="4" max="4" width="12.5" customWidth="1"/>
+    <col min="5" max="5" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:5" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="31"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="3" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32">
         <v>1</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="6"/>
-    </row>
-    <row r="4" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B5" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C5" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="2" t="s">
+      <c r="D5" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="34">
         <v>2</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B12" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="15" t="s">
+      <c r="C12" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="34">
         <v>3</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="33" t="s">
+      <c r="C16" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="33" t="s">
-        <v>46</v>
-      </c>
       <c r="B17" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="34">
         <v>4</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="15" t="s">
+      <c r="D19" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="33" t="s">
+      <c r="B20" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="18" t="s">
-        <v>50</v>
-      </c>
       <c r="C20" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="29" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="29" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="35">
         <v>5</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C21" s="17"/>
       <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="28"/>
-    </row>
-    <row r="22" spans="1:6" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E21" s="28"/>
+    </row>
+    <row r="22" spans="1:5" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B22" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="D22" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="25" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="B23" s="18" t="s">
+      <c r="C23" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="25" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D23" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E23" s="25" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="B24" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="C24" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="C24" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="25" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" s="29" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D24" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="29" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="35">
         <v>6</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C25" s="17"/>
       <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="28"/>
-    </row>
-    <row r="26" spans="1:6" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E25" s="28"/>
+    </row>
+    <row r="26" spans="1:5" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E26" s="25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="B26" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="25" t="s">
+      <c r="B27" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27" s="18"/>
+      <c r="D27" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E27" s="25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E28" s="25" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="B27" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="25" t="s">
+    <row r="29" spans="1:5" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D29" s="24"/>
+      <c r="E29" s="25" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="33" t="s">
-        <v>104</v>
-      </c>
-      <c r="B28" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="C28" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="25" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="33" t="s">
-        <v>111</v>
-      </c>
-      <c r="B29" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="C29" s="18" t="s">
+    <row r="30" spans="1:5" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="25" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="33" t="s">
+      <c r="B30" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="B30" s="18" t="s">
-        <v>115</v>
-      </c>
       <c r="C30" s="18"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="25" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D30" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E30" s="25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="B31" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="C31" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="C31" s="18" t="s">
+      <c r="D31" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E31" s="25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="33" t="s">
         <v>121</v>
       </c>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="25" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="33" t="s">
+      <c r="B32" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="C32" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="C32" s="39" t="s">
-        <v>124</v>
-      </c>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="25" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D32" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E32" s="25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="35">
         <v>7</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C33" s="15"/>
       <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="2"/>
-    </row>
-    <row r="34" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C34" s="15"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D34" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B35" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="C35" s="15" t="s">
+      <c r="D35" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="B36" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="B36" s="18" t="s">
+      <c r="C36" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C36" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="2" t="s">
+      <c r="D36" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="B37" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="33" t="s">
-        <v>107</v>
-      </c>
-      <c r="B37" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="35">
         <v>6</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C38" s="15"/>
       <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="2"/>
-    </row>
-    <row r="39" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="B39" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="2" t="s">
+      <c r="B40" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="15" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="B40" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C40" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D40" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="35">
         <v>8</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C41" s="15"/>
       <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="2"/>
-    </row>
-    <row r="42" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E41" s="2"/>
+    </row>
+    <row r="42" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="B42" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C42" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="2" t="s">
+      <c r="B43" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="B43" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="C43" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" s="29" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" s="29" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="35">
         <v>9</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C44" s="17"/>
       <c r="D44" s="27"/>
-      <c r="E44" s="27"/>
-      <c r="F44" s="28"/>
-    </row>
-    <row r="45" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E44" s="28"/>
+    </row>
+    <row r="45" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C45" s="15"/>
+      <c r="D45" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="B45" s="15" t="s">
+      <c r="B46" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C45" s="15"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="2" t="s">
+      <c r="C46" s="15"/>
+      <c r="D46" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="33" t="s">
+    <row r="47" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A47" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="B46" s="15" t="s">
+      <c r="B47" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="C46" s="15"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A47" s="33" t="s">
-        <v>79</v>
-      </c>
-      <c r="B47" s="15" t="s">
+      <c r="C47" s="15"/>
+      <c r="D47" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="B48" s="17" t="s">
         <v>82</v>
-      </c>
-      <c r="C47" s="15"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="35" t="s">
-        <v>96</v>
-      </c>
-      <c r="B48" s="17" t="s">
-        <v>83</v>
       </c>
       <c r="C48" s="17"/>
       <c r="D48" s="27"/>
-      <c r="E48" s="27"/>
-      <c r="F48" s="28"/>
-    </row>
-    <row r="49" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E48" s="28"/>
+    </row>
+    <row r="49" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A49" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C49" s="15"/>
+      <c r="D49" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="B49" s="15" t="s">
+      <c r="B50" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="C49" s="15"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="2" t="s">
+      <c r="C50" s="15"/>
+      <c r="D50" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E50" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="33" t="s">
+    <row r="51" spans="1:5" s="29" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="B50" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="C50" s="15"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" s="29" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="35" t="s">
-        <v>99</v>
-      </c>
       <c r="B51" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C51" s="17"/>
       <c r="D51" s="27"/>
-      <c r="E51" s="27"/>
-      <c r="F51" s="28"/>
-    </row>
-    <row r="52" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E51" s="28"/>
+    </row>
+    <row r="52" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A52" s="33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C52" s="19">
         <v>43760</v>
       </c>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="D52" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A53" s="33" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C53" s="19">
         <v>43781</v>
       </c>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="D53" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A54" s="33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C54" s="19">
         <v>43797</v>
       </c>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D54" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="36"/>
       <c r="B55" s="15"/>
       <c r="C55" s="15"/>
       <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="2"/>
-    </row>
-    <row r="56" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E55" s="2"/>
+    </row>
+    <row r="56" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="36"/>
       <c r="B56" s="15"/>
       <c r="C56" s="15"/>
       <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="2"/>
-    </row>
-    <row r="57" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E56" s="2"/>
+    </row>
+    <row r="57" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="36"/>
       <c r="B57" s="15"/>
       <c r="C57" s="15"/>
       <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="2"/>
-    </row>
-    <row r="58" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E57" s="2"/>
+    </row>
+    <row r="58" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="36"/>
       <c r="B58" s="15"/>
       <c r="C58" s="15"/>
       <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="2"/>
-    </row>
-    <row r="59" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E58" s="2"/>
+    </row>
+    <row r="59" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="36"/>
       <c r="B59" s="15"/>
       <c r="C59" s="15"/>
       <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="2"/>
-    </row>
-    <row r="60" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E59" s="2"/>
+    </row>
+    <row r="60" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="36"/>
       <c r="B60" s="15"/>
       <c r="C60" s="15"/>
       <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="2"/>
-    </row>
-    <row r="61" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E60" s="2"/>
+    </row>
+    <row r="61" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="36"/>
       <c r="B61" s="15"/>
       <c r="C61" s="15"/>
       <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="2"/>
-    </row>
-    <row r="62" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E61" s="2"/>
+    </row>
+    <row r="62" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="36"/>
       <c r="B62" s="15"/>
       <c r="C62" s="15"/>
       <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-      <c r="F62" s="2"/>
-    </row>
-    <row r="63" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E62" s="2"/>
+    </row>
+    <row r="63" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="36"/>
       <c r="B63" s="15"/>
       <c r="C63" s="15"/>
       <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="2"/>
-    </row>
-    <row r="64" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E63" s="2"/>
+    </row>
+    <row r="64" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="36"/>
       <c r="B64" s="20"/>
       <c r="C64" s="15"/>
       <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
-      <c r="F64" s="2"/>
-    </row>
-    <row r="65" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E64" s="2"/>
+    </row>
+    <row r="65" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="37"/>
       <c r="B65" s="21"/>
       <c r="C65" s="22"/>
       <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="4"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E65" s="4"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C66" s="12"/>
     </row>
   </sheetData>
@@ -2079,7 +2101,7 @@
     <oddFooter>&amp;L&amp;"Calibri (Textkörper),Standard"&amp;K00-034Seite ____/_____&amp;C&amp;"Calibri (Textkörper),Standard"&amp;K00-034Heidenheim, den _________&amp;R&amp;"Calibri (Textkörper),Standard"&amp;K00-034erstellt von: ______________</oddFooter>
   </headerFooter>
   <colBreaks count="1" manualBreakCount="1">
-    <brk id="6" max="1048575" man="1"/>
+    <brk id="5" max="1048575" man="1"/>
   </colBreaks>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Morphologischer Kasten, Anforderungsliste im Projektbericht eingefügt
</commit_message>
<xml_diff>
--- a/RB-Blessing/Anforderungsliste.xlsx
+++ b/RB-Blessing/Anforderungsliste.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\langohra.tmb18\Documents\GitHub\KE3\RB-Blessing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hofmannt.tmb18\Documents\GitHub\KE3\RB-Blessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094EE418-EAEF-4AE7-9CA8-DE12D5464970}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB2AA7C8-EFC6-44B5-8FFE-814F0AA21E58}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -621,7 +621,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -781,10 +781,34 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
         <color auto="1"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -794,10 +818,34 @@
       <left style="thin">
         <color auto="1"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color auto="1"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -813,8 +861,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -829,21 +875,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -862,11 +899,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -897,6 +930,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1182,12 +1242,12 @@
   <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.625" style="38" customWidth="1"/>
+    <col min="1" max="1" width="6.625" style="29" customWidth="1"/>
     <col min="2" max="2" width="25.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44.875" customWidth="1"/>
     <col min="4" max="4" width="12.5" customWidth="1"/>
@@ -1195,904 +1255,918 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="9" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="31"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="8"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="32">
+      <c r="A3" s="23">
         <v>1</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="36"/>
     </row>
     <row r="4" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="31" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="31" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="31" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="31" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="31" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="31" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="34">
+      <c r="A10" s="25">
         <v>2</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="2"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="39"/>
     </row>
     <row r="11" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="31" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="31" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="31" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="34">
+      <c r="A14" s="25">
         <v>3</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="2"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="39"/>
     </row>
     <row r="15" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="31" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="31" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="31" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="34">
+      <c r="A18" s="25">
         <v>4</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="2"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="39"/>
     </row>
     <row r="19" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="31" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="31" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="29" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="35">
+    <row r="21" spans="1:5" s="20" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="26">
         <v>5</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="28"/>
-    </row>
-    <row r="22" spans="1:5" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="33" t="s">
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="39"/>
+    </row>
+    <row r="22" spans="1:5" s="19" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="E22" s="25" t="s">
+      <c r="E22" s="32" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="33" t="s">
+    <row r="23" spans="1:5" s="19" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="E23" s="25" t="s">
+      <c r="E23" s="32" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="33" t="s">
+    <row r="24" spans="1:5" s="19" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="E24" s="25" t="s">
+      <c r="E24" s="32" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="29" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="35">
+    <row r="25" spans="1:5" s="20" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="26">
         <v>6</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="37" t="s">
         <v>127</v>
       </c>
-      <c r="C25" s="17"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="28"/>
-    </row>
-    <row r="26" spans="1:5" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="33" t="s">
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="39"/>
+    </row>
+    <row r="26" spans="1:5" s="19" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="E26" s="25" t="s">
+      <c r="E26" s="32" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="33" t="s">
+    <row r="27" spans="1:5" s="19" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="1" t="s">
+      <c r="C27" s="13"/>
+      <c r="D27" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="E27" s="25" t="s">
+      <c r="E27" s="32" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="33" t="s">
+    <row r="28" spans="1:5" s="19" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="C28" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="E28" s="25" t="s">
+      <c r="E28" s="32" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="33" t="s">
+    <row r="29" spans="1:5" s="19" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="B29" s="18" t="s">
+      <c r="B29" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="D29" s="24"/>
-      <c r="E29" s="25" t="s">
+      <c r="D29" s="33"/>
+      <c r="E29" s="32" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="33" t="s">
+    <row r="30" spans="1:5" s="19" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="1" t="s">
+      <c r="C30" s="13"/>
+      <c r="D30" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="E30" s="25" t="s">
+      <c r="E30" s="32" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="33" t="s">
+    <row r="31" spans="1:5" s="19" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="C31" s="18" t="s">
+      <c r="C31" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="E31" s="25" t="s">
+      <c r="E31" s="32" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="26" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="33" t="s">
+    <row r="32" spans="1:5" s="19" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="C32" s="39" t="s">
+      <c r="C32" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="E32" s="25" t="s">
+      <c r="E32" s="32" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="35">
+      <c r="A33" s="26">
         <v>7</v>
       </c>
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="15"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="2"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="39"/>
     </row>
     <row r="34" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="33" t="s">
+      <c r="A34" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C34" s="15"/>
-      <c r="D34" s="1" t="s">
+      <c r="C34" s="11"/>
+      <c r="D34" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E34" s="31" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="33" t="s">
+      <c r="A35" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="B35" s="18" t="s">
+      <c r="B35" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="C35" s="15" t="s">
+      <c r="C35" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E35" s="31" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="33" t="s">
+      <c r="A36" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C36" s="15" t="s">
+      <c r="C36" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="E36" s="31" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="33" t="s">
+      <c r="A37" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="B37" s="18" t="s">
+      <c r="B37" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="C37" s="15" t="s">
+      <c r="C37" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="E37" s="31" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="35">
+      <c r="A38" s="26">
         <v>6</v>
       </c>
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="C38" s="15"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="2"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="39"/>
     </row>
     <row r="39" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="33" t="s">
+      <c r="A39" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="B39" s="18" t="s">
+      <c r="B39" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="C39" s="15" t="s">
+      <c r="C39" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="E39" s="31" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="33" t="s">
+      <c r="A40" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="B40" s="18" t="s">
+      <c r="B40" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="15" t="s">
+      <c r="C40" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D40" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="E40" s="31" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="35">
+      <c r="A41" s="26">
         <v>8</v>
       </c>
-      <c r="B41" s="17" t="s">
+      <c r="B41" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="C41" s="15"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="2"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="39"/>
     </row>
     <row r="42" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="33" t="s">
+      <c r="A42" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="B42" s="15" t="s">
+      <c r="B42" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C42" s="15" t="s">
+      <c r="C42" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D42" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="E42" s="31" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="33" t="s">
+      <c r="A43" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="15" t="s">
+      <c r="C43" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D43" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="E43" s="31" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="29" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="35">
+    <row r="44" spans="1:5" s="20" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="26">
         <v>9</v>
       </c>
-      <c r="B44" s="17" t="s">
+      <c r="B44" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="C44" s="17"/>
-      <c r="D44" s="27"/>
-      <c r="E44" s="28"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="39"/>
     </row>
     <row r="45" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="33" t="s">
+      <c r="A45" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="C45" s="15"/>
-      <c r="D45" s="1" t="s">
+      <c r="C45" s="11"/>
+      <c r="D45" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="E45" s="31" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="33" t="s">
+      <c r="A46" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="B46" s="15" t="s">
+      <c r="B46" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C46" s="15"/>
-      <c r="D46" s="1" t="s">
+      <c r="C46" s="11"/>
+      <c r="D46" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="E46" s="31" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A47" s="33" t="s">
+      <c r="A47" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="B47" s="15" t="s">
+      <c r="B47" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="C47" s="15"/>
-      <c r="D47" s="1" t="s">
+      <c r="C47" s="11"/>
+      <c r="D47" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="E47" s="31" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="48" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="35" t="s">
+    <row r="48" spans="1:5" s="20" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="B48" s="17" t="s">
+      <c r="B48" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="C48" s="17"/>
-      <c r="D48" s="27"/>
-      <c r="E48" s="28"/>
+      <c r="C48" s="38"/>
+      <c r="D48" s="38"/>
+      <c r="E48" s="39"/>
     </row>
     <row r="49" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="33" t="s">
+      <c r="A49" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="B49" s="15" t="s">
+      <c r="B49" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="C49" s="15"/>
-      <c r="D49" s="1" t="s">
+      <c r="C49" s="11"/>
+      <c r="D49" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="E49" s="31" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="33" t="s">
+      <c r="A50" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="B50" s="15" t="s">
+      <c r="B50" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="C50" s="15"/>
-      <c r="D50" s="1" t="s">
+      <c r="C50" s="11"/>
+      <c r="D50" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="E50" s="2" t="s">
+      <c r="E50" s="31" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="29" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="35" t="s">
+    <row r="51" spans="1:5" s="20" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="B51" s="17" t="s">
+      <c r="B51" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="C51" s="17"/>
-      <c r="D51" s="27"/>
-      <c r="E51" s="28"/>
+      <c r="C51" s="38"/>
+      <c r="D51" s="38"/>
+      <c r="E51" s="39"/>
     </row>
     <row r="52" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="33" t="s">
+      <c r="A52" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="B52" s="15" t="s">
+      <c r="B52" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C52" s="19">
+      <c r="C52" s="14">
         <v>43760</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D52" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="E52" s="2" t="s">
+      <c r="E52" s="31" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A53" s="33" t="s">
+      <c r="A53" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="B53" s="15" t="s">
+      <c r="B53" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C53" s="19">
+      <c r="C53" s="14">
         <v>43781</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D53" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="E53" s="2" t="s">
+      <c r="E53" s="31" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A54" s="33" t="s">
+      <c r="A54" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="B54" s="15" t="s">
+      <c r="B54" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C54" s="19">
+      <c r="C54" s="14">
         <v>43797</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D54" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="E54" s="31" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="36"/>
-      <c r="B55" s="15"/>
-      <c r="C55" s="15"/>
+      <c r="A55" s="27"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
       <c r="D55" s="1"/>
       <c r="E55" s="2"/>
     </row>
     <row r="56" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="36"/>
-      <c r="B56" s="15"/>
-      <c r="C56" s="15"/>
+      <c r="A56" s="27"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="11"/>
       <c r="D56" s="1"/>
       <c r="E56" s="2"/>
     </row>
     <row r="57" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="36"/>
-      <c r="B57" s="15"/>
-      <c r="C57" s="15"/>
+      <c r="A57" s="27"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="11"/>
       <c r="D57" s="1"/>
       <c r="E57" s="2"/>
     </row>
     <row r="58" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="36"/>
-      <c r="B58" s="15"/>
-      <c r="C58" s="15"/>
+      <c r="A58" s="27"/>
+      <c r="B58" s="11"/>
+      <c r="C58" s="11"/>
       <c r="D58" s="1"/>
       <c r="E58" s="2"/>
     </row>
     <row r="59" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="36"/>
-      <c r="B59" s="15"/>
-      <c r="C59" s="15"/>
+      <c r="A59" s="27"/>
+      <c r="B59" s="11"/>
+      <c r="C59" s="11"/>
       <c r="D59" s="1"/>
       <c r="E59" s="2"/>
     </row>
     <row r="60" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="36"/>
-      <c r="B60" s="15"/>
-      <c r="C60" s="15"/>
+      <c r="A60" s="27"/>
+      <c r="B60" s="11"/>
+      <c r="C60" s="11"/>
       <c r="D60" s="1"/>
       <c r="E60" s="2"/>
     </row>
     <row r="61" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="36"/>
-      <c r="B61" s="15"/>
-      <c r="C61" s="15"/>
+      <c r="A61" s="27"/>
+      <c r="B61" s="11"/>
+      <c r="C61" s="11"/>
       <c r="D61" s="1"/>
       <c r="E61" s="2"/>
     </row>
     <row r="62" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="36"/>
-      <c r="B62" s="15"/>
-      <c r="C62" s="15"/>
+      <c r="A62" s="27"/>
+      <c r="B62" s="11"/>
+      <c r="C62" s="11"/>
       <c r="D62" s="1"/>
       <c r="E62" s="2"/>
     </row>
     <row r="63" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="36"/>
-      <c r="B63" s="15"/>
-      <c r="C63" s="15"/>
+      <c r="A63" s="27"/>
+      <c r="B63" s="11"/>
+      <c r="C63" s="11"/>
       <c r="D63" s="1"/>
       <c r="E63" s="2"/>
     </row>
     <row r="64" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="36"/>
-      <c r="B64" s="20"/>
-      <c r="C64" s="15"/>
+      <c r="A64" s="27"/>
+      <c r="B64" s="15"/>
+      <c r="C64" s="11"/>
       <c r="D64" s="1"/>
       <c r="E64" s="2"/>
     </row>
     <row r="65" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="37"/>
-      <c r="B65" s="21"/>
-      <c r="C65" s="22"/>
+      <c r="A65" s="28"/>
+      <c r="B65" s="16"/>
+      <c r="C65" s="17"/>
       <c r="D65" s="3"/>
       <c r="E65" s="4"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C66" s="12"/>
+      <c r="C66" s="10"/>
     </row>
   </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B51:E51"/>
+    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B21:E21"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="1.0236220472440944" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="69" orientation="portrait" copies="10" r:id="rId1"/>

</xml_diff>